<commit_message>
complete the description of Lhub_SRS_2.3.2 ID
</commit_message>
<xml_diff>
--- a/Lhub_SRS_CRS_V1.xlsx
+++ b/Lhub_SRS_CRS_V1.xlsx
@@ -15,7 +15,6 @@
     <sheet name="CRS VS SRS" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -96,11 +95,6 @@
     <t>Lhub_SRS_2.5.1</t>
   </si>
   <si>
-    <t xml:space="preserve">•      As a user I want to have  Browser (chrome or Firefox ) so that I can open the web site
-•      As a user I want to open the website on operating system (windows) so that I want to 
-</t>
-  </si>
-  <si>
     <t>Learning Hub is a web platform</t>
   </si>
   <si>
@@ -156,12 +150,6 @@
     <t>The user can get notifications whenever any article is added in that category by any user</t>
   </si>
   <si>
-    <t xml:space="preserve">•  As a user I want to get notifications from the category I have followed so that I know that new article is added
-•  As a user I can search for any article or a word so that I can find the article or a word it contains.
-•  As a user I have the ability to rate other users’ articles so that there will be interaction between users
- </t>
-  </si>
-  <si>
     <t xml:space="preserve"> •   As a user I can follow specific category so that I can catch up with new articles added to that category</t>
   </si>
   <si>
@@ -169,6 +157,16 @@
   </si>
   <si>
     <t>•   As an admin I have to review each article uploaded by the user so that I could accept or reject it before publishing online</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•      As a user I want to have  Browser (chrome or Firefox ) so that I can open the web site
+•      As a user, I want to open the website on operating system (windows) so that I can see the articles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•  As a user I want to get notifications from the category I have followed so that I know that    new article is added
+•  As a user I can search for any article or a word so that I can find the article or a word it contains.
+•  As a user I have the ability to rate other users’ articles so that there will be interaction between users
+ </t>
   </si>
 </sst>
 </file>
@@ -656,8 +654,8 @@
   </sheetPr>
   <dimension ref="A1:V999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -706,13 +704,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -741,10 +739,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -765,7 +763,7 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="4" spans="1:22" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="55.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
@@ -776,7 +774,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -797,7 +795,7 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="91.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
@@ -805,10 +803,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -837,10 +835,10 @@
         <v>14</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
@@ -866,13 +864,13 @@
         <v>15</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
@@ -904,7 +902,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -930,13 +928,13 @@
         <v>19</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -968,7 +966,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>

</xml_diff>